<commit_message>
them download file excel
</commit_message>
<xml_diff>
--- a/static/uploads/Book1.xlsx
+++ b/static/uploads/Book1.xlsx
@@ -14,24 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>Work Center</t>
   </si>
   <si>
-    <t>REEDEDLINE</t>
+    <t>PACKING</t>
   </si>
   <si>
     <t>From</t>
   </si>
   <si>
-    <t>2024-05-08</t>
+    <t>2024-05-13</t>
   </si>
   <si>
     <t>To</t>
   </si>
   <si>
-    <t>2024-05-21</t>
+    <t>2024-05-19</t>
   </si>
   <si>
     <t>Ngày giờ nhập</t>
@@ -41,6 +41,414 @@
   </si>
   <si>
     <t>Manhr</t>
+  </si>
+  <si>
+    <t>2024-05-20 02:41:06</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>792</t>
+  </si>
+  <si>
+    <t>2024-05-19 12:48:59</t>
+  </si>
+  <si>
+    <t>6081</t>
+  </si>
+  <si>
+    <t>2024-05-19 09:01:51</t>
+  </si>
+  <si>
+    <t>15911</t>
+  </si>
+  <si>
+    <t>2024-05-19 08:52:20</t>
+  </si>
+  <si>
+    <t>52565</t>
+  </si>
+  <si>
+    <t>2024-05-19 08:49:43</t>
+  </si>
+  <si>
+    <t>24680</t>
+  </si>
+  <si>
+    <t>2024-05-19 06:30:42</t>
+  </si>
+  <si>
+    <t>10901</t>
+  </si>
+  <si>
+    <t>2024-05-19 02:26:35</t>
+  </si>
+  <si>
+    <t>5820</t>
+  </si>
+  <si>
+    <t>2024-05-18 08:59:54</t>
+  </si>
+  <si>
+    <t>1460</t>
+  </si>
+  <si>
+    <t>2024-05-18 08:50:56</t>
+  </si>
+  <si>
+    <t>13195</t>
+  </si>
+  <si>
+    <t>2024-05-18 08:37:34</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>2024-05-18 08:20:14</t>
+  </si>
+  <si>
+    <t>928</t>
+  </si>
+  <si>
+    <t>2024-05-18 07:44:20</t>
+  </si>
+  <si>
+    <t>9267</t>
+  </si>
+  <si>
+    <t>2024-05-18 07:24:46</t>
+  </si>
+  <si>
+    <t>21273</t>
+  </si>
+  <si>
+    <t>2024-05-18 07:00:39</t>
+  </si>
+  <si>
+    <t>6670</t>
+  </si>
+  <si>
+    <t>2024-05-18 06:59:58</t>
+  </si>
+  <si>
+    <t>16114</t>
+  </si>
+  <si>
+    <t>2024-05-18 03:50:33</t>
+  </si>
+  <si>
+    <t>4441</t>
+  </si>
+  <si>
+    <t>2024-05-18 03:45:10</t>
+  </si>
+  <si>
+    <t>13945</t>
+  </si>
+  <si>
+    <t>2024-05-18 00:25:07</t>
+  </si>
+  <si>
+    <t>737</t>
+  </si>
+  <si>
+    <t>2024-05-17 14:38:36</t>
+  </si>
+  <si>
+    <t>1024</t>
+  </si>
+  <si>
+    <t>2024-05-17 13:36:02</t>
+  </si>
+  <si>
+    <t>7993</t>
+  </si>
+  <si>
+    <t>2024-05-17 13:34:53</t>
+  </si>
+  <si>
+    <t>10764</t>
+  </si>
+  <si>
+    <t>2024-05-17 13:34:44</t>
+  </si>
+  <si>
+    <t>12509</t>
+  </si>
+  <si>
+    <t>2024-05-17 10:28:07</t>
+  </si>
+  <si>
+    <t>6983</t>
+  </si>
+  <si>
+    <t>2024-05-17 10:26:44</t>
+  </si>
+  <si>
+    <t>8853</t>
+  </si>
+  <si>
+    <t>2024-05-17 07:50:11</t>
+  </si>
+  <si>
+    <t>11932</t>
+  </si>
+  <si>
+    <t>2024-05-17 07:18:58</t>
+  </si>
+  <si>
+    <t>6599</t>
+  </si>
+  <si>
+    <t>2024-05-17 06:30:29</t>
+  </si>
+  <si>
+    <t>10370</t>
+  </si>
+  <si>
+    <t>2024-05-17 05:49:30</t>
+  </si>
+  <si>
+    <t>9450</t>
+  </si>
+  <si>
+    <t>2024-05-17 05:05:23</t>
+  </si>
+  <si>
+    <t>17413</t>
+  </si>
+  <si>
+    <t>2024-05-16 13:14:23</t>
+  </si>
+  <si>
+    <t>14775</t>
+  </si>
+  <si>
+    <t>2024-05-16 11:57:38</t>
+  </si>
+  <si>
+    <t>8675</t>
+  </si>
+  <si>
+    <t>2024-05-16 11:35:32</t>
+  </si>
+  <si>
+    <t>20424</t>
+  </si>
+  <si>
+    <t>2024-05-16 11:33:40</t>
+  </si>
+  <si>
+    <t>21647</t>
+  </si>
+  <si>
+    <t>2024-05-16 10:44:07</t>
+  </si>
+  <si>
+    <t>1148</t>
+  </si>
+  <si>
+    <t>2024-05-16 08:51:18</t>
+  </si>
+  <si>
+    <t>20493</t>
+  </si>
+  <si>
+    <t>2024-05-16 08:07:46</t>
+  </si>
+  <si>
+    <t>8502</t>
+  </si>
+  <si>
+    <t>2024-05-16 05:53:10</t>
+  </si>
+  <si>
+    <t>13687</t>
+  </si>
+  <si>
+    <t>2024-05-16 05:53:00</t>
+  </si>
+  <si>
+    <t>14910</t>
+  </si>
+  <si>
+    <t>2024-05-16 05:21:10</t>
+  </si>
+  <si>
+    <t>30991</t>
+  </si>
+  <si>
+    <t>2024-05-16 04:04:19</t>
+  </si>
+  <si>
+    <t>1393</t>
+  </si>
+  <si>
+    <t>2024-05-16 00:19:50</t>
+  </si>
+  <si>
+    <t>8876</t>
+  </si>
+  <si>
+    <t>2024-05-15 13:39:36</t>
+  </si>
+  <si>
+    <t>14262</t>
+  </si>
+  <si>
+    <t>2024-05-15 13:37:34</t>
+  </si>
+  <si>
+    <t>5147</t>
+  </si>
+  <si>
+    <t>2024-05-15 13:35:30</t>
+  </si>
+  <si>
+    <t>13944</t>
+  </si>
+  <si>
+    <t>2024-05-15 11:41:18</t>
+  </si>
+  <si>
+    <t>10991</t>
+  </si>
+  <si>
+    <t>2024-05-15 11:38:49</t>
+  </si>
+  <si>
+    <t>9115</t>
+  </si>
+  <si>
+    <t>2024-05-15 10:44:45</t>
+  </si>
+  <si>
+    <t>13520</t>
+  </si>
+  <si>
+    <t>2024-05-15 10:14:20</t>
+  </si>
+  <si>
+    <t>3991</t>
+  </si>
+  <si>
+    <t>2024-05-15 08:59:45</t>
+  </si>
+  <si>
+    <t>12418</t>
+  </si>
+  <si>
+    <t>2024-05-15 08:56:05</t>
+  </si>
+  <si>
+    <t>4327</t>
+  </si>
+  <si>
+    <t>2024-05-15 07:41:59</t>
+  </si>
+  <si>
+    <t>19284</t>
+  </si>
+  <si>
+    <t>2024-05-15 07:19:25</t>
+  </si>
+  <si>
+    <t>9076</t>
+  </si>
+  <si>
+    <t>2024-05-15 04:45:45</t>
+  </si>
+  <si>
+    <t>11896</t>
+  </si>
+  <si>
+    <t>2024-05-15 03:37:10</t>
+  </si>
+  <si>
+    <t>1251</t>
+  </si>
+  <si>
+    <t>2024-05-15 02:26:30</t>
+  </si>
+  <si>
+    <t>2343</t>
+  </si>
+  <si>
+    <t>2024-05-15 02:26:05</t>
+  </si>
+  <si>
+    <t>8877</t>
+  </si>
+  <si>
+    <t>2024-05-15 07:47:54</t>
+  </si>
+  <si>
+    <t>43312</t>
+  </si>
+  <si>
+    <t>2024-05-15 06:02:19</t>
+  </si>
+  <si>
+    <t>1372</t>
+  </si>
+  <si>
+    <t>2024-05-15 00:57:52</t>
+  </si>
+  <si>
+    <t>78514</t>
+  </si>
+  <si>
+    <t>2024-05-15 00:45:54</t>
+  </si>
+  <si>
+    <t>8142</t>
+  </si>
+  <si>
+    <t>2024-05-14 06:54:27</t>
+  </si>
+  <si>
+    <t>6698</t>
+  </si>
+  <si>
+    <t>2024-05-14 00:32:35</t>
+  </si>
+  <si>
+    <t>24199</t>
+  </si>
+  <si>
+    <t>2024-05-14 03:18:21</t>
+  </si>
+  <si>
+    <t>1431</t>
+  </si>
+  <si>
+    <t>2024-05-14 00:33:37</t>
+  </si>
+  <si>
+    <t>75301</t>
+  </si>
+  <si>
+    <t>2024-05-14 00:32:59</t>
+  </si>
+  <si>
+    <t>2024-05-14 00:30:58</t>
+  </si>
+  <si>
+    <t>31275</t>
+  </si>
+  <si>
+    <t>2024-05-13 08:35:51</t>
+  </si>
+  <si>
+    <t>7980</t>
+  </si>
+  <si>
+    <t>2024-05-13 06:06:50</t>
+  </si>
+  <si>
+    <t>10139</t>
   </si>
 </sst>
 </file>
@@ -358,9 +766,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -375,6 +789,765 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
them so luong vao xem efficienct
</commit_message>
<xml_diff>
--- a/static/uploads/Book1.xlsx
+++ b/static/uploads/Book1.xlsx
@@ -14,30 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Work Center</t>
   </si>
   <si>
-    <t>ASSEMBLY</t>
+    <t>PACKING</t>
   </si>
   <si>
     <t>From</t>
   </si>
   <si>
-    <t>2024-05-22</t>
+    <t>2024-06-01</t>
   </si>
   <si>
     <t>To</t>
   </si>
   <si>
-    <t>2024-05-23</t>
-  </si>
-  <si>
     <t>Ngày giờ nhập</t>
   </si>
   <si>
-    <t>Số Lượng</t>
+    <t>Sản Lượng</t>
   </si>
   <si>
     <t>Manhr</t>
@@ -49,10 +46,10 @@
     <t>Loại Hàng</t>
   </si>
   <si>
-    <t>2024-05-23 15:13:49</t>
-  </si>
-  <si>
-    <t>38818</t>
+    <t>Số lượng (pcs)</t>
+  </si>
+  <si>
+    <t>2024-06-03 01:01:15</t>
   </si>
   <si>
     <t>0</t>
@@ -64,151 +61,103 @@
     <t>RH</t>
   </si>
   <si>
-    <t>2024-05-23 15:04:14</t>
-  </si>
-  <si>
-    <t>13355</t>
+    <t>88</t>
+  </si>
+  <si>
+    <t>2024-06-03 01:00:47</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2024-05-23 15:03:03</t>
-  </si>
-  <si>
-    <t>5401</t>
+    <t>93</t>
+  </si>
+  <si>
+    <t>2024-06-03 00:57:27</t>
   </si>
   <si>
     <t>BRAND</t>
   </si>
   <si>
-    <t>2024-05-23 10:22:48</t>
-  </si>
-  <si>
-    <t>17826</t>
-  </si>
-  <si>
-    <t>2024-05-23 10:04:07</t>
-  </si>
-  <si>
-    <t>11920</t>
-  </si>
-  <si>
-    <t>2024-05-23 10:03:17</t>
-  </si>
-  <si>
-    <t>29883</t>
-  </si>
-  <si>
-    <t>2024-05-23 09:33:22</t>
-  </si>
-  <si>
-    <t>4045</t>
+    <t>57</t>
+  </si>
+  <si>
+    <t>2024-06-02 06:34:28</t>
+  </si>
+  <si>
+    <t>9421</t>
+  </si>
+  <si>
+    <t>2024-06-02 06:20:44</t>
+  </si>
+  <si>
+    <t>1274</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2024-05-23 08:03:50</t>
-  </si>
-  <si>
-    <t>10521</t>
-  </si>
-  <si>
-    <t>2024-05-23 04:41:32</t>
-  </si>
-  <si>
-    <t>10598</t>
-  </si>
-  <si>
-    <t>2024-05-23 03:22:04</t>
-  </si>
-  <si>
-    <t>12237</t>
-  </si>
-  <si>
-    <t>2024-05-23 03:16:30</t>
-  </si>
-  <si>
-    <t>5266</t>
-  </si>
-  <si>
-    <t>2024-05-23 03:16:20</t>
-  </si>
-  <si>
-    <t>1848</t>
-  </si>
-  <si>
-    <t>2024-05-22 16:45:56</t>
-  </si>
-  <si>
-    <t>3973</t>
-  </si>
-  <si>
-    <t>2024-05-22 15:29:05</t>
-  </si>
-  <si>
-    <t>20000</t>
-  </si>
-  <si>
-    <t>2024-05-22 15:19:00</t>
-  </si>
-  <si>
-    <t>18000</t>
-  </si>
-  <si>
-    <t>2024-05-22 14:56:59</t>
-  </si>
-  <si>
-    <t>5448</t>
-  </si>
-  <si>
-    <t>2024-05-22 10:08:04</t>
-  </si>
-  <si>
-    <t>24972</t>
-  </si>
-  <si>
-    <t>2024-05-22 09:44:04</t>
-  </si>
-  <si>
-    <t>4202</t>
-  </si>
-  <si>
-    <t>2024-05-22 07:57:14</t>
-  </si>
-  <si>
-    <t>18163</t>
-  </si>
-  <si>
-    <t>2024-05-22 07:51:49</t>
-  </si>
-  <si>
-    <t>11397</t>
-  </si>
-  <si>
-    <t>2024-05-22 05:33:29</t>
-  </si>
-  <si>
-    <t>4896</t>
-  </si>
-  <si>
-    <t>2024-05-22 05:20:02</t>
-  </si>
-  <si>
-    <t>13685</t>
-  </si>
-  <si>
-    <t>2024-05-22 02:36:57</t>
-  </si>
-  <si>
-    <t>11180</t>
-  </si>
-  <si>
-    <t>2024-05-22 02:34:10</t>
-  </si>
-  <si>
-    <t>9675</t>
+    <t>2024-06-01 12:27:48</t>
+  </si>
+  <si>
+    <t>6786</t>
+  </si>
+  <si>
+    <t>2024-06-01 12:27:26</t>
+  </si>
+  <si>
+    <t>8985</t>
+  </si>
+  <si>
+    <t>2024-06-01 11:54:44</t>
+  </si>
+  <si>
+    <t>6252</t>
+  </si>
+  <si>
+    <t>2024-06-01 11:29:26</t>
+  </si>
+  <si>
+    <t>7699</t>
+  </si>
+  <si>
+    <t>2024-06-01 09:42:46</t>
+  </si>
+  <si>
+    <t>11118</t>
+  </si>
+  <si>
+    <t>2024-06-01 08:42:13</t>
+  </si>
+  <si>
+    <t>6037</t>
+  </si>
+  <si>
+    <t>2024-06-01 07:42:35</t>
+  </si>
+  <si>
+    <t>10568</t>
+  </si>
+  <si>
+    <t>2024-06-01 07:36:14</t>
+  </si>
+  <si>
+    <t>2507</t>
+  </si>
+  <si>
+    <t>2024-06-01 07:35:42</t>
+  </si>
+  <si>
+    <t>8230</t>
+  </si>
+  <si>
+    <t>2024-06-01 07:35:27</t>
+  </si>
+  <si>
+    <t>2024-06-01 04:28:10</t>
+  </si>
+  <si>
+    <t>15796</t>
   </si>
 </sst>
 </file>
@@ -535,23 +484,26 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -563,12 +515,15 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -577,16 +532,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -594,15 +552,18 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -614,13 +575,16 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -628,50 +592,59 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -682,13 +655,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -699,13 +675,16 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -716,13 +695,16 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -733,13 +715,16 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -750,13 +735,16 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -764,16 +752,19 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -784,13 +775,16 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -798,169 +792,39 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
       <c r="E18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>